<commit_message>
Added basic testing functions for calc_pier_reaction.
Finished testing basic functionality of the calc_pier_reaction function.
Used excel functionality to independently check the output values. Saved a
copy of the excel files in the test folder.

Added an additional testing function for the calc_load_and_loc to test the
"rtl" functionality. The "ltr" was already tested.

All tests are successful.
</commit_message>
<xml_diff>
--- a/test/calc_load_and_loc.xlsx
+++ b/test/calc_load_and_loc.xlsx
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,15 +524,15 @@
         <v>98</v>
       </c>
       <c r="D8" s="4">
-        <f>IF(AND(C8&gt;=$C$3, C8&lt;=$C$4), B8, 0)</f>
+        <f t="shared" ref="D8:D25" si="0">IF(AND(C8&gt;=$C$3, C8&lt;=$C$4), B8, 0)</f>
         <v>40</v>
       </c>
       <c r="E8" s="4">
-        <f>IF(AND(C8&gt;=$C$3, C8&lt;=$C$2),B8,0)</f>
+        <f t="shared" ref="E8:E25" si="1">IF(AND(C8&gt;=$C$3, C8&lt;=$C$2),B8,0)</f>
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <f>IF(AND(C8&gt;=$C$2, C8&lt;=$C$4), B8, 0)</f>
+        <f t="shared" ref="F8:F25" si="2">IF(AND(C8&gt;=$C$2, C8&lt;=$C$4), B8, 0)</f>
         <v>40</v>
       </c>
       <c r="G8" s="4">
@@ -559,27 +559,27 @@
         <v>90</v>
       </c>
       <c r="D9" s="4">
-        <f>IF(AND(C9&gt;=$C$3, C9&lt;=$C$4), B9, 0)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="E9" s="4">
-        <f>IF(AND(C9&gt;=$C$3, C9&lt;=$C$2),B9,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F9" s="4">
-        <f>IF(AND(C9&gt;=$C$2, C9&lt;=$C$4), B9, 0)</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="G9" s="4">
-        <f t="shared" ref="G9:G25" si="0">D9*C9</f>
+        <f t="shared" ref="G9:G25" si="3">D9*C9</f>
         <v>7200</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" ref="H9:H25" si="1">E9*C9</f>
+        <f t="shared" ref="H9:H25" si="4">E9*C9</f>
         <v>0</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" ref="I9:I25" si="2">F9*C9</f>
+        <f t="shared" ref="I9:I25" si="5">F9*C9</f>
         <v>7200</v>
       </c>
     </row>
@@ -594,27 +594,27 @@
         <v>85</v>
       </c>
       <c r="D10" s="4">
-        <f>IF(AND(C10&gt;=$C$3, C10&lt;=$C$4), B10, 0)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="E10" s="4">
-        <f>IF(AND(C10&gt;=$C$3, C10&lt;=$C$2),B10,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F10" s="4">
-        <f>IF(AND(C10&gt;=$C$2, C10&lt;=$C$4), B10, 0)</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6800</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6800</v>
       </c>
     </row>
@@ -629,27 +629,27 @@
         <v>80</v>
       </c>
       <c r="D11" s="4">
-        <f>IF(AND(C11&gt;=$C$3, C11&lt;=$C$4), B11, 0)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="E11" s="4">
-        <f>IF(AND(C11&gt;=$C$3, C11&lt;=$C$2),B11,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F11" s="4">
-        <f>IF(AND(C11&gt;=$C$2, C11&lt;=$C$4), B11, 0)</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6400</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6400</v>
       </c>
     </row>
@@ -664,27 +664,27 @@
         <v>75</v>
       </c>
       <c r="D12" s="4">
-        <f>IF(AND(C12&gt;=$C$3, C12&lt;=$C$4), B12, 0)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="E12" s="4">
-        <f>IF(AND(C12&gt;=$C$3, C12&lt;=$C$2),B12,0)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="F12" s="4">
-        <f>IF(AND(C12&gt;=$C$2, C12&lt;=$C$4), B12, 0)</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6000</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6000</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6000</v>
       </c>
     </row>
@@ -699,27 +699,27 @@
         <v>66</v>
       </c>
       <c r="D13" s="4">
-        <f>IF(AND(C13&gt;=$C$3, C13&lt;=$C$4), B13, 0)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="E13" s="4">
-        <f>IF(AND(C13&gt;=$C$3, C13&lt;=$C$2),B13,0)</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="F13" s="4">
-        <f>IF(AND(C13&gt;=$C$2, C13&lt;=$C$4), B13, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3432</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3432</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -734,27 +734,27 @@
         <v>61</v>
       </c>
       <c r="D14" s="4">
-        <f>IF(AND(C14&gt;=$C$3, C14&lt;=$C$4), B14, 0)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="E14" s="4">
-        <f>IF(AND(C14&gt;=$C$3, C14&lt;=$C$2),B14,0)</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="F14" s="4">
-        <f>IF(AND(C14&gt;=$C$2, C14&lt;=$C$4), B14, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3172</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3172</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -769,27 +769,27 @@
         <v>55</v>
       </c>
       <c r="D15" s="4">
-        <f>IF(AND(C15&gt;=$C$3, C15&lt;=$C$4), B15, 0)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="E15" s="4">
-        <f>IF(AND(C15&gt;=$C$3, C15&lt;=$C$2),B15,0)</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="F15" s="4">
-        <f>IF(AND(C15&gt;=$C$2, C15&lt;=$C$4), B15, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2860</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2860</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -804,27 +804,27 @@
         <v>50</v>
       </c>
       <c r="D16" s="4">
-        <f>IF(AND(C16&gt;=$C$3, C16&lt;=$C$4), B16, 0)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="E16" s="4">
-        <f>IF(AND(C16&gt;=$C$3, C16&lt;=$C$2),B16,0)</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="F16" s="4">
-        <f>IF(AND(C16&gt;=$C$2, C16&lt;=$C$4), B16, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2600</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2600</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -839,27 +839,27 @@
         <v>42</v>
       </c>
       <c r="D17" s="4">
-        <f>IF(AND(C17&gt;=$C$3, C17&lt;=$C$4), B17, 0)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="E17" s="4">
-        <f>IF(AND(C17&gt;=$C$3, C17&lt;=$C$2),B17,0)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="F17" s="4">
-        <f>IF(AND(C17&gt;=$C$2, C17&lt;=$C$4), B17, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1680</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1680</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -874,27 +874,27 @@
         <v>34</v>
       </c>
       <c r="D18" s="4">
-        <f>IF(AND(C18&gt;=$C$3, C18&lt;=$C$4), B18, 0)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="E18" s="4">
-        <f>IF(AND(C18&gt;=$C$3, C18&lt;=$C$2),B18,0)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="F18" s="4">
-        <f>IF(AND(C18&gt;=$C$2, C18&lt;=$C$4), B18, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2720</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2720</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -909,27 +909,27 @@
         <v>29</v>
       </c>
       <c r="D19" s="4">
-        <f>IF(AND(C19&gt;=$C$3, C19&lt;=$C$4), B19, 0)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="E19" s="4">
-        <f>IF(AND(C19&gt;=$C$3, C19&lt;=$C$2),B19,0)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="F19" s="4">
-        <f>IF(AND(C19&gt;=$C$2, C19&lt;=$C$4), B19, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2320</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2320</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -944,27 +944,27 @@
         <v>24</v>
       </c>
       <c r="D20" s="4">
-        <f>IF(AND(C20&gt;=$C$3, C20&lt;=$C$4), B20, 0)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="E20" s="4">
-        <f>IF(AND(C20&gt;=$C$3, C20&lt;=$C$2),B20,0)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="F20" s="4">
-        <f>IF(AND(C20&gt;=$C$2, C20&lt;=$C$4), B20, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1920</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1920</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -979,27 +979,27 @@
         <v>19</v>
       </c>
       <c r="D21" s="4">
-        <f>IF(AND(C21&gt;=$C$3, C21&lt;=$C$4), B21, 0)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="E21" s="4">
-        <f>IF(AND(C21&gt;=$C$3, C21&lt;=$C$2),B21,0)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="F21" s="4">
-        <f>IF(AND(C21&gt;=$C$2, C21&lt;=$C$4), B21, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1520</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1520</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1014,27 +1014,27 @@
         <v>10</v>
       </c>
       <c r="D22" s="4">
-        <f>IF(AND(C22&gt;=$C$3, C22&lt;=$C$4), B22, 0)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="E22" s="4">
-        <f>IF(AND(C22&gt;=$C$3, C22&lt;=$C$2),B22,0)</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="F22" s="4">
-        <f>IF(AND(C22&gt;=$C$2, C22&lt;=$C$4), B22, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>520</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>520</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1049,27 +1049,27 @@
         <v>5</v>
       </c>
       <c r="D23" s="4">
-        <f>IF(AND(C23&gt;=$C$3, C23&lt;=$C$4), B23, 0)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="E23" s="4">
-        <f>IF(AND(C23&gt;=$C$3, C23&lt;=$C$2),B23,0)</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="F23" s="4">
-        <f>IF(AND(C23&gt;=$C$2, C23&lt;=$C$4), B23, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>260</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>260</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1084,27 +1084,27 @@
         <v>-1</v>
       </c>
       <c r="D24" s="4">
-        <f>IF(AND(C24&gt;=$C$3, C24&lt;=$C$4), B24, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E24" s="4">
-        <f>IF(AND(C24&gt;=$C$3, C24&lt;=$C$2),B24,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F24" s="4">
-        <f>IF(AND(C24&gt;=$C$2, C24&lt;=$C$4), B24, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1119,27 +1119,27 @@
         <v>-6</v>
       </c>
       <c r="D25" s="4">
-        <f>IF(AND(C25&gt;=$C$3, C25&lt;=$C$4), B25, 0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E25" s="4">
-        <f>IF(AND(C25&gt;=$C$3, C25&lt;=$C$2),B25,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F25" s="4">
-        <f>IF(AND(C25&gt;=$C$2, C25&lt;=$C$4), B25, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1163,23 +1163,23 @@
         <v>1032</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" ref="E27:I27" si="3">SUM(E8:E25)</f>
+        <f t="shared" ref="E27:I27" si="6">SUM(E8:E25)</f>
         <v>752</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>360</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>53324</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>29004</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>30320</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed excel file inputs for testing.
</commit_message>
<xml_diff>
--- a/test/calc_load_and_loc.xlsx
+++ b/test/calc_load_and_loc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16530" windowHeight="8970"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16530" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +521,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="5">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" ref="D8:D25" si="0">IF(AND(C8&gt;=$C$3, C8&lt;=$C$4), B8, 0)</f>
@@ -529,23 +529,23 @@
       </c>
       <c r="E8" s="4">
         <f t="shared" ref="E8:E25" si="1">IF(AND(C8&gt;=$C$3, C8&lt;=$C$2),B8,0)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" ref="F8:F25" si="2">IF(AND(C8&gt;=$C$2, C8&lt;=$C$4), B8, 0)</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
         <f>D8*C8</f>
-        <v>3920</v>
+        <v>760</v>
       </c>
       <c r="H8" s="4">
         <f>E8*C8</f>
-        <v>0</v>
+        <v>760</v>
       </c>
       <c r="I8" s="4">
         <f>F8*C8</f>
-        <v>3920</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>80</v>
       </c>
       <c r="C9" s="5">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
@@ -564,23 +564,23 @@
       </c>
       <c r="E9" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" ref="G9:G25" si="3">D9*C9</f>
-        <v>7200</v>
+        <v>2160</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" ref="H9:H25" si="4">E9*C9</f>
-        <v>0</v>
+        <v>2160</v>
       </c>
       <c r="I9" s="4">
         <f t="shared" ref="I9:I25" si="5">F9*C9</f>
-        <v>7200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -591,7 +591,7 @@
         <v>80</v>
       </c>
       <c r="C10" s="5">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
@@ -599,23 +599,23 @@
       </c>
       <c r="E10" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="3"/>
-        <v>6800</v>
+        <v>2560</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2560</v>
       </c>
       <c r="I10" s="4">
         <f t="shared" si="5"/>
-        <v>6800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
         <v>80</v>
       </c>
       <c r="C11" s="5">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="0"/>
@@ -634,23 +634,23 @@
       </c>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="3"/>
-        <v>6400</v>
+        <v>2960</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2960</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="5"/>
-        <v>6400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>80</v>
       </c>
       <c r="C12" s="5">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="0"/>
@@ -673,19 +673,19 @@
       </c>
       <c r="F12" s="4">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="3"/>
-        <v>6000</v>
+        <v>3360</v>
       </c>
       <c r="H12" s="4">
         <f t="shared" si="4"/>
-        <v>6000</v>
+        <v>3360</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="5"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -696,7 +696,7 @@
         <v>52</v>
       </c>
       <c r="C13" s="5">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="0"/>
@@ -712,11 +712,11 @@
       </c>
       <c r="G13" s="4">
         <f t="shared" si="3"/>
-        <v>3432</v>
+        <v>2652</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="4"/>
-        <v>3432</v>
+        <v>2652</v>
       </c>
       <c r="I13" s="4">
         <f t="shared" si="5"/>
@@ -731,7 +731,7 @@
         <v>52</v>
       </c>
       <c r="C14" s="5">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="0"/>
@@ -747,11 +747,11 @@
       </c>
       <c r="G14" s="4">
         <f t="shared" si="3"/>
-        <v>3172</v>
+        <v>2912</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" si="4"/>
-        <v>3172</v>
+        <v>2912</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="5"/>
@@ -766,7 +766,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="5">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="0"/>
@@ -782,11 +782,11 @@
       </c>
       <c r="G15" s="4">
         <f t="shared" si="3"/>
-        <v>2860</v>
+        <v>3224</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="4"/>
-        <v>2860</v>
+        <v>3224</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="5"/>
@@ -801,7 +801,7 @@
         <v>52</v>
       </c>
       <c r="C16" s="5">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="0"/>
@@ -817,11 +817,11 @@
       </c>
       <c r="G16" s="4">
         <f t="shared" si="3"/>
-        <v>2600</v>
+        <v>3484</v>
       </c>
       <c r="H16" s="4">
         <f t="shared" si="4"/>
-        <v>2600</v>
+        <v>3484</v>
       </c>
       <c r="I16" s="4">
         <f t="shared" si="5"/>
@@ -836,7 +836,7 @@
         <v>40</v>
       </c>
       <c r="C17" s="5">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="0"/>
@@ -848,19 +848,19 @@
       </c>
       <c r="F17" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" si="3"/>
-        <v>1680</v>
+        <v>3000</v>
       </c>
       <c r="H17" s="4">
         <f t="shared" si="4"/>
-        <v>1680</v>
+        <v>3000</v>
       </c>
       <c r="I17" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -871,7 +871,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="5">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="0"/>
@@ -879,23 +879,23 @@
       </c>
       <c r="E18" s="4">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G18" s="4">
         <f t="shared" si="3"/>
-        <v>2720</v>
+        <v>6640</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" si="4"/>
-        <v>2720</v>
+        <v>0</v>
       </c>
       <c r="I18" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>6640</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>80</v>
       </c>
       <c r="C19" s="5">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="0"/>
@@ -914,23 +914,23 @@
       </c>
       <c r="E19" s="4">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="3"/>
-        <v>2320</v>
+        <v>7040</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="4"/>
-        <v>2320</v>
+        <v>0</v>
       </c>
       <c r="I19" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7040</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -941,7 +941,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="5">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="0"/>
@@ -949,23 +949,23 @@
       </c>
       <c r="E20" s="4">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F20" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="3"/>
-        <v>1920</v>
+        <v>7440</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="4"/>
-        <v>1920</v>
+        <v>0</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7440</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -976,7 +976,7 @@
         <v>80</v>
       </c>
       <c r="C21" s="5">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="0"/>
@@ -984,23 +984,23 @@
       </c>
       <c r="E21" s="4">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="3"/>
-        <v>1520</v>
+        <v>7840</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="4"/>
-        <v>1520</v>
+        <v>0</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7840</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1011,15 +1011,15 @@
         <v>52</v>
       </c>
       <c r="C22" s="5">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="F22" s="4">
         <f t="shared" si="2"/>
@@ -1027,11 +1027,11 @@
       </c>
       <c r="G22" s="4">
         <f t="shared" si="3"/>
-        <v>520</v>
+        <v>0</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="4"/>
-        <v>520</v>
+        <v>0</v>
       </c>
       <c r="I22" s="4">
         <f t="shared" si="5"/>
@@ -1046,15 +1046,15 @@
         <v>52</v>
       </c>
       <c r="C23" s="5">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" si="2"/>
@@ -1062,11 +1062,11 @@
       </c>
       <c r="G23" s="4">
         <f t="shared" si="3"/>
-        <v>260</v>
+        <v>0</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="4"/>
-        <v>260</v>
+        <v>0</v>
       </c>
       <c r="I23" s="4">
         <f t="shared" si="5"/>
@@ -1081,7 +1081,7 @@
         <v>52</v>
       </c>
       <c r="C24" s="5">
-        <v>-1</v>
+        <v>118</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="0"/>
@@ -1116,7 +1116,7 @@
         <v>52</v>
       </c>
       <c r="C25" s="5">
-        <v>-6</v>
+        <v>123</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
@@ -1160,11 +1160,11 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4">
         <f>SUM(D8:D25)</f>
-        <v>1032</v>
+        <v>928</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" ref="E27:I27" si="6">SUM(E8:E25)</f>
-        <v>752</v>
+        <v>608</v>
       </c>
       <c r="F27" s="4">
         <f t="shared" si="6"/>
@@ -1172,29 +1172,29 @@
       </c>
       <c r="G27" s="4">
         <f t="shared" si="6"/>
-        <v>53324</v>
+        <v>56032</v>
       </c>
       <c r="H27" s="4">
         <f t="shared" si="6"/>
-        <v>29004</v>
+        <v>27072</v>
       </c>
       <c r="I27" s="4">
         <f t="shared" si="6"/>
-        <v>30320</v>
+        <v>31960</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G29" s="3">
         <f>G27/D27</f>
-        <v>51.670542635658911</v>
+        <v>60.379310344827587</v>
       </c>
       <c r="H29" s="3">
         <f>H27/E27</f>
-        <v>38.569148936170215</v>
+        <v>44.526315789473685</v>
       </c>
       <c r="I29" s="3">
         <f>I27/F27</f>
-        <v>84.222222222222229</v>
+        <v>88.777777777777771</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="C31" s="2">
         <f>D27</f>
-        <v>1032</v>
+        <v>928</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="C32" s="1">
         <f>G29</f>
-        <v>51.670542635658911</v>
+        <v>60.379310344827587</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="C33" s="1">
         <f>E27</f>
-        <v>752</v>
+        <v>608</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="C34" s="1">
         <f>H29</f>
-        <v>38.569148936170215</v>
+        <v>44.526315789473685</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C36" s="1">
         <f>I29</f>
-        <v>84.222222222222229</v>
+        <v>88.777777777777771</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests for calc_reactions and calc_pier_reactions in span 2.
Added code for multiple new tests in span 2. Completed tests for
calc_reactions and calc_pier reactions with x=125 so it is testing the
functionality in span 2.

Four other tests have not been completed in span 2. calc_shear with direction ltr,
and calc_reactions, calc_pier_reactions, and calc_shear with direction rtl. The
basic code structure is there but the independent calculations have not been
completed to produce an independent answer for testing purposes.

Four tests fail.
</commit_message>
<xml_diff>
--- a/test/calc_load_and_loc.xlsx
+++ b/test/calc_load_and_loc.xlsx
@@ -69,11 +69,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -153,7 +152,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -175,10 +174,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -262,7 +257,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -282,7 +277,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>75</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,7 +285,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,7 +293,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -338,7 +333,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="D8" s="2" t="n">
         <f aca="false">IF(AND(C8&gt;=$C$3, C8&lt;=$C$4), B8, 0)</f>
@@ -373,7 +368,7 @@
         <v>80</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>123</v>
+        <v>173</v>
       </c>
       <c r="D9" s="2" t="n">
         <f aca="false">IF(AND(C9&gt;=$C$3, C9&lt;=$C$4), B9, 0)</f>
@@ -408,7 +403,7 @@
         <v>80</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>118</v>
+        <v>168</v>
       </c>
       <c r="D10" s="2" t="n">
         <f aca="false">IF(AND(C10&gt;=$C$3, C10&lt;=$C$4), B10, 0)</f>
@@ -443,7 +438,7 @@
         <v>80</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="D11" s="2" t="n">
         <f aca="false">IF(AND(C11&gt;=$C$3, C11&lt;=$C$4), B11, 0)</f>
@@ -478,7 +473,7 @@
         <v>80</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="D12" s="2" t="n">
         <f aca="false">IF(AND(C12&gt;=$C$3, C12&lt;=$C$4), B12, 0)</f>
@@ -513,7 +508,7 @@
         <v>52</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="D13" s="2" t="n">
         <f aca="false">IF(AND(C13&gt;=$C$3, C13&lt;=$C$4), B13, 0)</f>
@@ -529,7 +524,7 @@
       </c>
       <c r="G13" s="2" t="n">
         <f aca="false">D13*C13</f>
-        <v>5148</v>
+        <v>7748</v>
       </c>
       <c r="H13" s="2" t="n">
         <f aca="false">E13*C13</f>
@@ -537,7 +532,7 @@
       </c>
       <c r="I13" s="2" t="n">
         <f aca="false">F13*C13</f>
-        <v>5148</v>
+        <v>7748</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,7 +543,7 @@
         <v>52</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="D14" s="2" t="n">
         <f aca="false">IF(AND(C14&gt;=$C$3, C14&lt;=$C$4), B14, 0)</f>
@@ -564,7 +559,7 @@
       </c>
       <c r="G14" s="2" t="n">
         <f aca="false">D14*C14</f>
-        <v>4888</v>
+        <v>7488</v>
       </c>
       <c r="H14" s="2" t="n">
         <f aca="false">E14*C14</f>
@@ -572,7 +567,7 @@
       </c>
       <c r="I14" s="2" t="n">
         <f aca="false">F14*C14</f>
-        <v>4888</v>
+        <v>7488</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,7 +578,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="D15" s="2" t="n">
         <f aca="false">IF(AND(C15&gt;=$C$3, C15&lt;=$C$4), B15, 0)</f>
@@ -599,7 +594,7 @@
       </c>
       <c r="G15" s="2" t="n">
         <f aca="false">D15*C15</f>
-        <v>4576</v>
+        <v>7176</v>
       </c>
       <c r="H15" s="2" t="n">
         <f aca="false">E15*C15</f>
@@ -607,7 +602,7 @@
       </c>
       <c r="I15" s="2" t="n">
         <f aca="false">F15*C15</f>
-        <v>4576</v>
+        <v>7176</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -618,7 +613,7 @@
         <v>52</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="D16" s="2" t="n">
         <f aca="false">IF(AND(C16&gt;=$C$3, C16&lt;=$C$4), B16, 0)</f>
@@ -634,7 +629,7 @@
       </c>
       <c r="G16" s="2" t="n">
         <f aca="false">D16*C16</f>
-        <v>4316</v>
+        <v>6916</v>
       </c>
       <c r="H16" s="2" t="n">
         <f aca="false">E16*C16</f>
@@ -642,7 +637,7 @@
       </c>
       <c r="I16" s="2" t="n">
         <f aca="false">F16*C16</f>
-        <v>4316</v>
+        <v>6916</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,7 +648,7 @@
         <v>40</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="D17" s="2" t="n">
         <f aca="false">IF(AND(C17&gt;=$C$3, C17&lt;=$C$4), B17, 0)</f>
@@ -669,15 +664,15 @@
       </c>
       <c r="G17" s="2" t="n">
         <f aca="false">D17*C17</f>
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="H17" s="2" t="n">
         <f aca="false">E17*C17</f>
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="I17" s="2" t="n">
         <f aca="false">F17*C17</f>
-        <v>3000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,7 +683,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="D18" s="2" t="n">
         <f aca="false">IF(AND(C18&gt;=$C$3, C18&lt;=$C$4), B18, 0)</f>
@@ -704,11 +699,11 @@
       </c>
       <c r="G18" s="2" t="n">
         <f aca="false">D18*C18</f>
-        <v>5360</v>
+        <v>9360</v>
       </c>
       <c r="H18" s="2" t="n">
         <f aca="false">E18*C18</f>
-        <v>5360</v>
+        <v>9360</v>
       </c>
       <c r="I18" s="2" t="n">
         <f aca="false">F18*C18</f>
@@ -723,7 +718,7 @@
         <v>80</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="D19" s="2" t="n">
         <f aca="false">IF(AND(C19&gt;=$C$3, C19&lt;=$C$4), B19, 0)</f>
@@ -739,11 +734,11 @@
       </c>
       <c r="G19" s="2" t="n">
         <f aca="false">D19*C19</f>
-        <v>4960</v>
+        <v>8960</v>
       </c>
       <c r="H19" s="2" t="n">
         <f aca="false">E19*C19</f>
-        <v>4960</v>
+        <v>8960</v>
       </c>
       <c r="I19" s="2" t="n">
         <f aca="false">F19*C19</f>
@@ -758,7 +753,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="3" t="n">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="D20" s="2" t="n">
         <f aca="false">IF(AND(C20&gt;=$C$3, C20&lt;=$C$4), B20, 0)</f>
@@ -774,11 +769,11 @@
       </c>
       <c r="G20" s="2" t="n">
         <f aca="false">D20*C20</f>
-        <v>4560</v>
+        <v>8560</v>
       </c>
       <c r="H20" s="2" t="n">
         <f aca="false">E20*C20</f>
-        <v>4560</v>
+        <v>8560</v>
       </c>
       <c r="I20" s="2" t="n">
         <f aca="false">F20*C20</f>
@@ -793,7 +788,7 @@
         <v>80</v>
       </c>
       <c r="C21" s="3" t="n">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="D21" s="2" t="n">
         <f aca="false">IF(AND(C21&gt;=$C$3, C21&lt;=$C$4), B21, 0)</f>
@@ -809,11 +804,11 @@
       </c>
       <c r="G21" s="2" t="n">
         <f aca="false">D21*C21</f>
-        <v>4160</v>
+        <v>8160</v>
       </c>
       <c r="H21" s="2" t="n">
         <f aca="false">E21*C21</f>
-        <v>4160</v>
+        <v>8160</v>
       </c>
       <c r="I21" s="2" t="n">
         <f aca="false">F21*C21</f>
@@ -828,15 +823,15 @@
         <v>52</v>
       </c>
       <c r="C22" s="3" t="n">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="D22" s="2" t="n">
         <f aca="false">IF(AND(C22&gt;=$C$3, C22&lt;=$C$4), B22, 0)</f>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E22" s="2" t="n">
         <f aca="false">IF(AND(C22&gt;=$C$3, C22&lt;=$C$2),B22,0)</f>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">IF(AND(C22&gt;=$C$2, C22&lt;=$C$4), B22, 0)</f>
@@ -844,11 +839,11 @@
       </c>
       <c r="G22" s="2" t="n">
         <f aca="false">D22*C22</f>
-        <v>2236</v>
+        <v>0</v>
       </c>
       <c r="H22" s="2" t="n">
         <f aca="false">E22*C22</f>
-        <v>2236</v>
+        <v>0</v>
       </c>
       <c r="I22" s="2" t="n">
         <f aca="false">F22*C22</f>
@@ -863,15 +858,15 @@
         <v>52</v>
       </c>
       <c r="C23" s="3" t="n">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="D23" s="2" t="n">
         <f aca="false">IF(AND(C23&gt;=$C$3, C23&lt;=$C$4), B23, 0)</f>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2" t="n">
         <f aca="false">IF(AND(C23&gt;=$C$3, C23&lt;=$C$2),B23,0)</f>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="F23" s="2" t="n">
         <f aca="false">IF(AND(C23&gt;=$C$2, C23&lt;=$C$4), B23, 0)</f>
@@ -879,11 +874,11 @@
       </c>
       <c r="G23" s="2" t="n">
         <f aca="false">D23*C23</f>
-        <v>1976</v>
+        <v>0</v>
       </c>
       <c r="H23" s="2" t="n">
         <f aca="false">E23*C23</f>
-        <v>1976</v>
+        <v>0</v>
       </c>
       <c r="I23" s="2" t="n">
         <f aca="false">F23*C23</f>
@@ -898,15 +893,15 @@
         <v>52</v>
       </c>
       <c r="C24" s="3" t="n">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="D24" s="2" t="n">
         <f aca="false">IF(AND(C24&gt;=$C$3, C24&lt;=$C$4), B24, 0)</f>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E24" s="2" t="n">
         <f aca="false">IF(AND(C24&gt;=$C$3, C24&lt;=$C$2),B24,0)</f>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="F24" s="2" t="n">
         <f aca="false">IF(AND(C24&gt;=$C$2, C24&lt;=$C$4), B24, 0)</f>
@@ -914,11 +909,11 @@
       </c>
       <c r="G24" s="2" t="n">
         <f aca="false">D24*C24</f>
-        <v>1664</v>
+        <v>0</v>
       </c>
       <c r="H24" s="2" t="n">
         <f aca="false">E24*C24</f>
-        <v>1664</v>
+        <v>0</v>
       </c>
       <c r="I24" s="2" t="n">
         <f aca="false">F24*C24</f>
@@ -933,15 +928,15 @@
         <v>52</v>
       </c>
       <c r="C25" s="3" t="n">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="D25" s="2" t="n">
         <f aca="false">IF(AND(C25&gt;=$C$3, C25&lt;=$C$4), B25, 0)</f>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E25" s="2" t="n">
         <f aca="false">IF(AND(C25&gt;=$C$3, C25&lt;=$C$2),B25,0)</f>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="F25" s="2" t="n">
         <f aca="false">IF(AND(C25&gt;=$C$2, C25&lt;=$C$4), B25, 0)</f>
@@ -949,11 +944,11 @@
       </c>
       <c r="G25" s="2" t="n">
         <f aca="false">D25*C25</f>
-        <v>1404</v>
+        <v>0</v>
       </c>
       <c r="H25" s="2" t="n">
         <f aca="false">E25*C25</f>
-        <v>1404</v>
+        <v>0</v>
       </c>
       <c r="I25" s="2" t="n">
         <f aca="false">F25*C25</f>
@@ -977,11 +972,11 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="n">
         <f aca="false">SUM(D8:D25)</f>
-        <v>776</v>
+        <v>568</v>
       </c>
       <c r="E27" s="2" t="n">
         <f aca="false">SUM(E8:E25)</f>
-        <v>568</v>
+        <v>360</v>
       </c>
       <c r="F27" s="2" t="n">
         <f aca="false">SUM(F8:F25)</f>
@@ -989,29 +984,29 @@
       </c>
       <c r="G27" s="2" t="n">
         <f aca="false">SUM(G8:G25)</f>
-        <v>48248</v>
+        <v>69368</v>
       </c>
       <c r="H27" s="2" t="n">
         <f aca="false">SUM(H8:H25)</f>
-        <v>29320</v>
+        <v>40040</v>
       </c>
       <c r="I27" s="2" t="n">
         <f aca="false">SUM(I8:I25)</f>
-        <v>21928</v>
+        <v>34328</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G29" s="4" t="n">
         <f aca="false">G27/D27</f>
-        <v>62.1752577319588</v>
+        <v>122.12676056338</v>
       </c>
       <c r="H29" s="4" t="n">
         <f aca="false">H27/E27</f>
-        <v>51.6197183098592</v>
+        <v>111.222222222222</v>
       </c>
       <c r="I29" s="4" t="n">
         <f aca="false">I27/F27</f>
-        <v>88.4193548387097</v>
+        <v>138.41935483871</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1020,41 +1015,41 @@
       </c>
       <c r="C31" s="5" t="n">
         <f aca="false">D27</f>
-        <v>776</v>
+        <v>568</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="6" t="n">
+      <c r="C32" s="5" t="n">
         <f aca="false">G29</f>
-        <v>62.1752577319588</v>
+        <v>122.12676056338</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="6" t="n">
+      <c r="C33" s="5" t="n">
         <f aca="false">E27</f>
-        <v>568</v>
+        <v>360</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="6" t="n">
+      <c r="C34" s="5" t="n">
         <f aca="false">H29</f>
-        <v>51.6197183098592</v>
+        <v>111.222222222222</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="6" t="n">
+      <c r="C35" s="5" t="n">
         <f aca="false">F27</f>
         <v>248</v>
       </c>
@@ -1063,9 +1058,9 @@
       <c r="B36" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="6" t="n">
+      <c r="C36" s="5" t="n">
         <f aca="false">I29</f>
-        <v>88.4193548387097</v>
+        <v>138.41935483871</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished testing on span 2 for calc_shear, calc_reactions, calc_pier_reactions.
Tested ltr and rtl on span 2 at x = 125.

Started tests for calc_moment.

Moment tests do not pass. All other tests pass.
</commit_message>
<xml_diff>
--- a/test/calc_load_and_loc.xlsx
+++ b/test/calc_load_and_loc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="655" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="881" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -256,8 +256,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -277,7 +277,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>125</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -285,7 +285,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -293,7 +293,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,7 +333,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="D8" s="2" t="n">
         <f aca="false">IF(AND(C8&gt;=$C$3, C8&lt;=$C$4), B8, 0)</f>
@@ -368,7 +368,7 @@
         <v>80</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="D9" s="2" t="n">
         <f aca="false">IF(AND(C9&gt;=$C$3, C9&lt;=$C$4), B9, 0)</f>
@@ -403,7 +403,7 @@
         <v>80</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="D10" s="2" t="n">
         <f aca="false">IF(AND(C10&gt;=$C$3, C10&lt;=$C$4), B10, 0)</f>
@@ -438,7 +438,7 @@
         <v>80</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="D11" s="2" t="n">
         <f aca="false">IF(AND(C11&gt;=$C$3, C11&lt;=$C$4), B11, 0)</f>
@@ -473,7 +473,7 @@
         <v>80</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="D12" s="2" t="n">
         <f aca="false">IF(AND(C12&gt;=$C$3, C12&lt;=$C$4), B12, 0)</f>
@@ -508,7 +508,7 @@
         <v>52</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="D13" s="2" t="n">
         <f aca="false">IF(AND(C13&gt;=$C$3, C13&lt;=$C$4), B13, 0)</f>
@@ -524,7 +524,7 @@
       </c>
       <c r="G13" s="2" t="n">
         <f aca="false">D13*C13</f>
-        <v>7748</v>
+        <v>5148</v>
       </c>
       <c r="H13" s="2" t="n">
         <f aca="false">E13*C13</f>
@@ -532,7 +532,7 @@
       </c>
       <c r="I13" s="2" t="n">
         <f aca="false">F13*C13</f>
-        <v>7748</v>
+        <v>5148</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,7 +543,7 @@
         <v>52</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="D14" s="2" t="n">
         <f aca="false">IF(AND(C14&gt;=$C$3, C14&lt;=$C$4), B14, 0)</f>
@@ -559,7 +559,7 @@
       </c>
       <c r="G14" s="2" t="n">
         <f aca="false">D14*C14</f>
-        <v>7488</v>
+        <v>4888</v>
       </c>
       <c r="H14" s="2" t="n">
         <f aca="false">E14*C14</f>
@@ -567,7 +567,7 @@
       </c>
       <c r="I14" s="2" t="n">
         <f aca="false">F14*C14</f>
-        <v>7488</v>
+        <v>4888</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -578,7 +578,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="D15" s="2" t="n">
         <f aca="false">IF(AND(C15&gt;=$C$3, C15&lt;=$C$4), B15, 0)</f>
@@ -594,7 +594,7 @@
       </c>
       <c r="G15" s="2" t="n">
         <f aca="false">D15*C15</f>
-        <v>7176</v>
+        <v>4576</v>
       </c>
       <c r="H15" s="2" t="n">
         <f aca="false">E15*C15</f>
@@ -602,7 +602,7 @@
       </c>
       <c r="I15" s="2" t="n">
         <f aca="false">F15*C15</f>
-        <v>7176</v>
+        <v>4576</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,7 +613,7 @@
         <v>52</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="D16" s="2" t="n">
         <f aca="false">IF(AND(C16&gt;=$C$3, C16&lt;=$C$4), B16, 0)</f>
@@ -629,7 +629,7 @@
       </c>
       <c r="G16" s="2" t="n">
         <f aca="false">D16*C16</f>
-        <v>6916</v>
+        <v>4316</v>
       </c>
       <c r="H16" s="2" t="n">
         <f aca="false">E16*C16</f>
@@ -637,7 +637,7 @@
       </c>
       <c r="I16" s="2" t="n">
         <f aca="false">F16*C16</f>
-        <v>6916</v>
+        <v>4316</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -648,7 +648,7 @@
         <v>40</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="D17" s="2" t="n">
         <f aca="false">IF(AND(C17&gt;=$C$3, C17&lt;=$C$4), B17, 0)</f>
@@ -664,15 +664,15 @@
       </c>
       <c r="G17" s="2" t="n">
         <f aca="false">D17*C17</f>
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="H17" s="2" t="n">
         <f aca="false">E17*C17</f>
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="I17" s="2" t="n">
         <f aca="false">F17*C17</f>
-        <v>5000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -683,7 +683,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="D18" s="2" t="n">
         <f aca="false">IF(AND(C18&gt;=$C$3, C18&lt;=$C$4), B18, 0)</f>
@@ -699,11 +699,11 @@
       </c>
       <c r="G18" s="2" t="n">
         <f aca="false">D18*C18</f>
-        <v>9360</v>
+        <v>5360</v>
       </c>
       <c r="H18" s="2" t="n">
         <f aca="false">E18*C18</f>
-        <v>9360</v>
+        <v>5360</v>
       </c>
       <c r="I18" s="2" t="n">
         <f aca="false">F18*C18</f>
@@ -718,7 +718,7 @@
         <v>80</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="D19" s="2" t="n">
         <f aca="false">IF(AND(C19&gt;=$C$3, C19&lt;=$C$4), B19, 0)</f>
@@ -734,11 +734,11 @@
       </c>
       <c r="G19" s="2" t="n">
         <f aca="false">D19*C19</f>
-        <v>8960</v>
+        <v>4960</v>
       </c>
       <c r="H19" s="2" t="n">
         <f aca="false">E19*C19</f>
-        <v>8960</v>
+        <v>4960</v>
       </c>
       <c r="I19" s="2" t="n">
         <f aca="false">F19*C19</f>
@@ -753,7 +753,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="3" t="n">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="D20" s="2" t="n">
         <f aca="false">IF(AND(C20&gt;=$C$3, C20&lt;=$C$4), B20, 0)</f>
@@ -769,11 +769,11 @@
       </c>
       <c r="G20" s="2" t="n">
         <f aca="false">D20*C20</f>
-        <v>8560</v>
+        <v>4560</v>
       </c>
       <c r="H20" s="2" t="n">
         <f aca="false">E20*C20</f>
-        <v>8560</v>
+        <v>4560</v>
       </c>
       <c r="I20" s="2" t="n">
         <f aca="false">F20*C20</f>
@@ -788,7 +788,7 @@
         <v>80</v>
       </c>
       <c r="C21" s="3" t="n">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="D21" s="2" t="n">
         <f aca="false">IF(AND(C21&gt;=$C$3, C21&lt;=$C$4), B21, 0)</f>
@@ -804,11 +804,11 @@
       </c>
       <c r="G21" s="2" t="n">
         <f aca="false">D21*C21</f>
-        <v>8160</v>
+        <v>4160</v>
       </c>
       <c r="H21" s="2" t="n">
         <f aca="false">E21*C21</f>
-        <v>8160</v>
+        <v>4160</v>
       </c>
       <c r="I21" s="2" t="n">
         <f aca="false">F21*C21</f>
@@ -823,15 +823,15 @@
         <v>52</v>
       </c>
       <c r="C22" s="3" t="n">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="D22" s="2" t="n">
         <f aca="false">IF(AND(C22&gt;=$C$3, C22&lt;=$C$4), B22, 0)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E22" s="2" t="n">
         <f aca="false">IF(AND(C22&gt;=$C$3, C22&lt;=$C$2),B22,0)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">IF(AND(C22&gt;=$C$2, C22&lt;=$C$4), B22, 0)</f>
@@ -839,11 +839,11 @@
       </c>
       <c r="G22" s="2" t="n">
         <f aca="false">D22*C22</f>
-        <v>0</v>
+        <v>2236</v>
       </c>
       <c r="H22" s="2" t="n">
         <f aca="false">E22*C22</f>
-        <v>0</v>
+        <v>2236</v>
       </c>
       <c r="I22" s="2" t="n">
         <f aca="false">F22*C22</f>
@@ -858,15 +858,15 @@
         <v>52</v>
       </c>
       <c r="C23" s="3" t="n">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="D23" s="2" t="n">
         <f aca="false">IF(AND(C23&gt;=$C$3, C23&lt;=$C$4), B23, 0)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E23" s="2" t="n">
         <f aca="false">IF(AND(C23&gt;=$C$3, C23&lt;=$C$2),B23,0)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="F23" s="2" t="n">
         <f aca="false">IF(AND(C23&gt;=$C$2, C23&lt;=$C$4), B23, 0)</f>
@@ -874,11 +874,11 @@
       </c>
       <c r="G23" s="2" t="n">
         <f aca="false">D23*C23</f>
-        <v>0</v>
+        <v>1976</v>
       </c>
       <c r="H23" s="2" t="n">
         <f aca="false">E23*C23</f>
-        <v>0</v>
+        <v>1976</v>
       </c>
       <c r="I23" s="2" t="n">
         <f aca="false">F23*C23</f>
@@ -893,15 +893,15 @@
         <v>52</v>
       </c>
       <c r="C24" s="3" t="n">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="D24" s="2" t="n">
         <f aca="false">IF(AND(C24&gt;=$C$3, C24&lt;=$C$4), B24, 0)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E24" s="2" t="n">
         <f aca="false">IF(AND(C24&gt;=$C$3, C24&lt;=$C$2),B24,0)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="F24" s="2" t="n">
         <f aca="false">IF(AND(C24&gt;=$C$2, C24&lt;=$C$4), B24, 0)</f>
@@ -909,11 +909,11 @@
       </c>
       <c r="G24" s="2" t="n">
         <f aca="false">D24*C24</f>
-        <v>0</v>
+        <v>1664</v>
       </c>
       <c r="H24" s="2" t="n">
         <f aca="false">E24*C24</f>
-        <v>0</v>
+        <v>1664</v>
       </c>
       <c r="I24" s="2" t="n">
         <f aca="false">F24*C24</f>
@@ -928,15 +928,15 @@
         <v>52</v>
       </c>
       <c r="C25" s="3" t="n">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="D25" s="2" t="n">
         <f aca="false">IF(AND(C25&gt;=$C$3, C25&lt;=$C$4), B25, 0)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E25" s="2" t="n">
         <f aca="false">IF(AND(C25&gt;=$C$3, C25&lt;=$C$2),B25,0)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="F25" s="2" t="n">
         <f aca="false">IF(AND(C25&gt;=$C$2, C25&lt;=$C$4), B25, 0)</f>
@@ -944,11 +944,11 @@
       </c>
       <c r="G25" s="2" t="n">
         <f aca="false">D25*C25</f>
-        <v>0</v>
+        <v>1404</v>
       </c>
       <c r="H25" s="2" t="n">
         <f aca="false">E25*C25</f>
-        <v>0</v>
+        <v>1404</v>
       </c>
       <c r="I25" s="2" t="n">
         <f aca="false">F25*C25</f>
@@ -972,11 +972,11 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="n">
         <f aca="false">SUM(D8:D25)</f>
-        <v>568</v>
+        <v>776</v>
       </c>
       <c r="E27" s="2" t="n">
         <f aca="false">SUM(E8:E25)</f>
-        <v>360</v>
+        <v>568</v>
       </c>
       <c r="F27" s="2" t="n">
         <f aca="false">SUM(F8:F25)</f>
@@ -984,29 +984,29 @@
       </c>
       <c r="G27" s="2" t="n">
         <f aca="false">SUM(G8:G25)</f>
-        <v>69368</v>
+        <v>48248</v>
       </c>
       <c r="H27" s="2" t="n">
         <f aca="false">SUM(H8:H25)</f>
-        <v>40040</v>
+        <v>29320</v>
       </c>
       <c r="I27" s="2" t="n">
         <f aca="false">SUM(I8:I25)</f>
-        <v>34328</v>
+        <v>21928</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G29" s="4" t="n">
         <f aca="false">G27/D27</f>
-        <v>122.12676056338</v>
+        <v>62.1752577319588</v>
       </c>
       <c r="H29" s="4" t="n">
         <f aca="false">H27/E27</f>
-        <v>111.222222222222</v>
+        <v>51.6197183098592</v>
       </c>
       <c r="I29" s="4" t="n">
         <f aca="false">I27/F27</f>
-        <v>138.41935483871</v>
+        <v>88.4193548387097</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,7 +1015,7 @@
       </c>
       <c r="C31" s="5" t="n">
         <f aca="false">D27</f>
-        <v>568</v>
+        <v>776</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="C32" s="5" t="n">
         <f aca="false">G29</f>
-        <v>122.12676056338</v>
+        <v>62.1752577319588</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="C33" s="5" t="n">
         <f aca="false">E27</f>
-        <v>360</v>
+        <v>568</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1042,7 +1042,7 @@
       </c>
       <c r="C34" s="5" t="n">
         <f aca="false">H29</f>
-        <v>111.222222222222</v>
+        <v>51.6197183098592</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="C36" s="5" t="n">
         <f aca="false">I29</f>
-        <v>138.41935483871</v>
+        <v>88.4193548387097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>